<commit_message>
Replace 180R with 470R
</commit_message>
<xml_diff>
--- a/x-IMU3-SA-A2-PCB/Project Outputs for x-IMU3-SA-A2/BOM/Bill of Materials-x-IMU3-SA-A2.xlsx
+++ b/x-IMU3-SA-A2-PCB/Project Outputs for x-IMU3-SA-A2/BOM/Bill of Materials-x-IMU3-SA-A2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\x-io\Products\x-IMU3\x-IMU3-SA-A2\x-IMU3-SA-A2-PCB\Project Outputs for x-IMU3-SA-A2\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99E14E02-9675-4C71-811A-4D0BD7AFF310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{02F077EF-3ACB-4836-816F-085660B743F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34810" yWindow="4140" windowWidth="14340" windowHeight="15420" xr2:uid="{1C2F5D80-9289-475F-80A5-D6312C5EDDDA}"/>
+    <workbookView xWindow="-38280" yWindow="6270" windowWidth="24150" windowHeight="15270" xr2:uid="{ED9B1C17-7902-4667-9875-CF44C14D3F29}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-x-IMU3-SA-A2" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>R1, R2, R3</t>
   </si>
   <si>
-    <t>180R</t>
+    <t>470R</t>
   </si>
   <si>
     <t>Resistor 0402</t>
@@ -472,7 +472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF25C80F-ECDE-4BAA-B609-F61FCAA576F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3713925F-520F-40E2-97FC-9991D93EB236}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>